<commit_message>
Changes in Lab2 and Lab3
Added graph in Lab2_report and created Lab3 deliverables.
</commit_message>
<xml_diff>
--- a/Lab2/Lab2_graph.xlsx
+++ b/Lab2/Lab2_graph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="8595" windowHeight="7740"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="8595" windowHeight="7740" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -143,6 +143,12 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:name/>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$27</c:f>
@@ -327,11 +333,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="46336256"/>
-        <c:axId val="46333952"/>
+        <c:axId val="173917312"/>
+        <c:axId val="173919232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46336256"/>
+        <c:axId val="173917312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -364,12 +370,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46333952"/>
+        <c:crossAx val="173919232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46333952"/>
+        <c:axId val="173919232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -399,7 +405,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46336256"/>
+        <c:crossAx val="173917312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -468,6 +474,11 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet2!$B$2:$B$15</c:f>
@@ -580,11 +591,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98458240"/>
-        <c:axId val="98456704"/>
+        <c:axId val="173931904"/>
+        <c:axId val="138413568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98458240"/>
+        <c:axId val="173931904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -613,12 +624,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98456704"/>
+        <c:crossAx val="138413568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98456704"/>
+        <c:axId val="138413568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,7 +664,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98458240"/>
+        <c:crossAx val="173931904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -722,6 +733,11 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet3!$B$1:$B$5</c:f>
@@ -780,11 +796,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="171375232"/>
-        <c:axId val="171373696"/>
+        <c:axId val="138444160"/>
+        <c:axId val="138565120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="171375232"/>
+        <c:axId val="138444160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,12 +834,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171373696"/>
+        <c:crossAx val="138565120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="171373696"/>
+        <c:axId val="138565120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,7 +874,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171375232"/>
+        <c:crossAx val="138444160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -927,6 +943,11 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet4!$B$1:$B$6</c:f>
@@ -991,11 +1012,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="177908736"/>
-        <c:axId val="177907200"/>
+        <c:axId val="138535296"/>
+        <c:axId val="138537216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="177908736"/>
+        <c:axId val="138535296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1029,12 +1050,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="177907200"/>
+        <c:crossAx val="138537216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="177907200"/>
+        <c:axId val="138537216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1090,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="177908736"/>
+        <c:crossAx val="138535296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1138,6 +1159,11 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet5!$B$1:$B$6</c:f>
@@ -1202,11 +1228,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="180848512"/>
-        <c:axId val="180846976"/>
+        <c:axId val="138610944"/>
+        <c:axId val="138654080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="180848512"/>
+        <c:axId val="138610944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1240,12 +1266,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180846976"/>
+        <c:crossAx val="138654080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="180846976"/>
+        <c:axId val="138654080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1280,7 +1306,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="180848512"/>
+        <c:crossAx val="138610944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1761,7 +1787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -2405,7 +2431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>

</xml_diff>